<commit_message>
added 3 , 7 day prediction horizon
</commit_message>
<xml_diff>
--- a/FYP - documents/EvaluationMetrics.xlsx
+++ b/FYP - documents/EvaluationMetrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackyboy/Desktop/PythonCryptoPrediction/FYP - documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCD6E12-3B88-7B4B-A7A7-9B15B5732F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0111017F-7B1D-7A48-8A9C-484B4C7E124F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="1840" windowWidth="28040" windowHeight="16940" xr2:uid="{1F5488E5-3192-D841-9991-E440C7A2F77A}"/>
+    <workbookView xWindow="8560" yWindow="2500" windowWidth="28040" windowHeight="16940" xr2:uid="{1F5488E5-3192-D841-9991-E440C7A2F77A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="9">
   <si>
     <t>MSE</t>
   </si>
@@ -57,12 +57,18 @@
   <si>
     <t>ETH</t>
   </si>
+  <si>
+    <t>7 DAYS</t>
+  </si>
+  <si>
+    <t>3 DAYS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -76,18 +82,37 @@
       <name val="Courier New"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="13"/>
-      <color theme="1"/>
-      <name val="Inherit"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -102,10 +127,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,132 +448,357 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E556151-BDE4-9F47-9B26-B95EBB299ABF}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="F24" sqref="C19:F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="19">
-      <c r="A2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1">
         <v>400.29394625773699</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="19">
-      <c r="A3" t="s">
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1">
+        <v>17</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1">
+        <v>20</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="1">
+        <v>7.6994394668881902E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>1.2394851723296E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="19">
-      <c r="A4" t="s">
+      <c r="D3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1">
+        <v>9.8847343079662697E-2</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.11133216841190099</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.102723975940163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1">
         <v>31.693544123903798</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="D4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1">
+        <v>4.72142781246996</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5.6297019569337596</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="1">
+        <v>7.8884707129884199E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="D8" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="19">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="19">
-      <c r="A9" t="s">
-        <v>5</v>
+      <c r="G8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B9" s="1">
-        <v>9.8847343079662697E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="19">
-      <c r="A10" t="s">
-        <v>6</v>
+        <v>1985.9505545649399</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="1">
+        <v>41.5702518538994</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="1">
+        <v>44.564005145015201</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.18609756934455901</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B10" s="1">
-        <v>4.72142781246996</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+        <v>2.1269171126152502E-2</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.13019392683502601</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.14583953896715501</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0.134366188390414</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1">
+        <v>133.87429421036899</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1">
+        <v>10.9665591328139</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="1">
+        <v>11.570405965668099</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.17923261223487699</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="G14" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="19">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="19">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1">
-        <v>0.11133216841190099</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="19">
-      <c r="A15" t="s">
-        <v>6</v>
+      <c r="J14" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B15" s="1">
-        <v>5.6297019569337596</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="19">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="1">
-        <v>7.6994394668881902E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="19">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="1">
-        <v>0.102723975940163</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="19">
-      <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="1">
-        <v>7.8884707129884199E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="17">
-      <c r="E27" s="2"/>
+        <v>2862.5306011223602</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1">
+        <v>49.7729157085002</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="1">
+        <v>53.502622376126197</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.22378378125815501</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1">
+        <v>5.24047222607689E-2</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.21597612916980399</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.22892077725879001</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0.22159300499051901</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1">
+        <v>370.45436813191901</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="1">
+        <v>18.723967361973799</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="1">
+        <v>19.247191175127799</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0.30632725853061199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="E29" s="1"/>
+      <c r="G29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>